<commit_message>
Added According to mark comments
</commit_message>
<xml_diff>
--- a/DataTillDate.xlsx
+++ b/DataTillDate.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="DataTillDate" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -843,9 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -874,1447 +872,1447 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42052</v>
+        <v>36860</v>
       </c>
       <c r="B2">
-        <v>199.51529410000001</v>
+        <v>415.49381820000002</v>
       </c>
       <c r="C2">
-        <v>421.74</v>
+        <v>392.17</v>
       </c>
       <c r="D2">
-        <v>72.5</v>
+        <v>106.8</v>
       </c>
       <c r="E2">
-        <v>70.400000000000006</v>
+        <v>112.7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42035</v>
+        <v>36891</v>
       </c>
       <c r="B3">
-        <v>202.3148387</v>
+        <v>206.46219350000001</v>
       </c>
       <c r="C3">
-        <v>422.2</v>
+        <v>392.42</v>
       </c>
       <c r="D3">
-        <v>67</v>
+        <v>104.4</v>
       </c>
       <c r="E3">
-        <v>72.8</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>42004</v>
+        <v>36922</v>
       </c>
       <c r="B4">
-        <v>201.62425809999999</v>
+        <v>202.27690319999999</v>
       </c>
       <c r="C4">
-        <v>421.66500000000002</v>
+        <v>392.46</v>
       </c>
       <c r="D4">
-        <v>78</v>
+        <v>95.6</v>
       </c>
       <c r="E4">
-        <v>81.599999999999994</v>
+        <v>108.7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41973</v>
+        <v>36950</v>
       </c>
       <c r="B5">
-        <v>236.732</v>
+        <v>201.38228570000001</v>
       </c>
       <c r="C5">
-        <v>421.13</v>
+        <v>392.5</v>
       </c>
       <c r="D5">
-        <v>70.099999999999994</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="E5">
-        <v>78.2</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41943</v>
+        <v>36978</v>
       </c>
       <c r="B6">
-        <v>241.18038709999999</v>
+        <v>189.35885709999999</v>
       </c>
       <c r="C6">
-        <v>421.83</v>
+        <v>393.17</v>
       </c>
       <c r="D6">
-        <v>60.6</v>
+        <v>113.5</v>
       </c>
       <c r="E6">
-        <v>83.4</v>
+        <v>104.8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41912</v>
+        <v>37011</v>
       </c>
       <c r="B7">
-        <v>255.61680000000001</v>
+        <v>262.74568420000003</v>
       </c>
       <c r="C7">
-        <v>421.91</v>
+        <v>393.57</v>
       </c>
       <c r="D7">
-        <v>87.6</v>
+        <v>107.7</v>
       </c>
       <c r="E7">
-        <v>74.8</v>
+        <v>107.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41882</v>
+        <v>37042</v>
       </c>
       <c r="B8">
-        <v>259.5852903</v>
+        <v>165.94620689999999</v>
       </c>
       <c r="C8">
-        <v>420.94</v>
+        <v>393.85</v>
       </c>
       <c r="D8">
-        <v>74.599999999999994</v>
+        <v>96.6</v>
       </c>
       <c r="E8">
-        <v>76.2</v>
+        <v>108.6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41851</v>
+        <v>37072</v>
       </c>
       <c r="B9">
-        <v>252.98219349999999</v>
+        <v>200.13120000000001</v>
       </c>
       <c r="C9">
-        <v>420.86</v>
+        <v>394.57</v>
       </c>
       <c r="D9">
-        <v>72.400000000000006</v>
+        <v>134</v>
       </c>
       <c r="E9">
-        <v>78.599999999999994</v>
+        <v>109.8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41820</v>
+        <v>37103</v>
       </c>
       <c r="B10">
-        <v>249.8898667</v>
+        <v>218.56258059999999</v>
       </c>
       <c r="C10">
-        <v>421.48</v>
+        <v>394.24</v>
       </c>
       <c r="D10">
-        <v>71</v>
+        <v>81.8</v>
       </c>
       <c r="E10">
-        <v>79.7</v>
+        <v>111.7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41790</v>
+        <v>37134</v>
       </c>
       <c r="B11">
-        <v>319.72129030000002</v>
+        <v>260.2905806</v>
       </c>
       <c r="C11">
-        <v>421.41</v>
+        <v>394.73</v>
       </c>
       <c r="D11">
-        <v>75.2</v>
+        <v>106.4</v>
       </c>
       <c r="E11">
-        <v>80.5</v>
+        <v>113.6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41759</v>
+        <v>37164</v>
       </c>
       <c r="B12">
-        <v>242.14453330000001</v>
+        <v>274.27972410000001</v>
       </c>
       <c r="C12">
-        <v>421.29</v>
+        <v>395.13</v>
       </c>
       <c r="D12">
-        <v>84.7</v>
+        <v>150.69999999999999</v>
       </c>
       <c r="E12">
-        <v>81.900000000000006</v>
+        <v>114.1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41729</v>
+        <v>37195</v>
       </c>
       <c r="B13">
-        <v>249.322</v>
+        <v>205.17446150000001</v>
       </c>
       <c r="C13">
-        <v>421.48</v>
+        <v>394.06</v>
       </c>
       <c r="D13">
-        <v>91.9</v>
+        <v>125.5</v>
       </c>
       <c r="E13">
-        <v>80.8</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41698</v>
+        <v>37225</v>
       </c>
       <c r="B14">
-        <v>195.16085709999999</v>
+        <v>313.12639999999999</v>
       </c>
       <c r="C14">
-        <v>421.24</v>
+        <v>394.66</v>
       </c>
       <c r="D14">
-        <v>102.3</v>
+        <v>106.5</v>
       </c>
       <c r="E14">
-        <v>78.3</v>
+        <v>115.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41670</v>
+        <v>37256</v>
       </c>
       <c r="B15">
-        <v>242.15690319999999</v>
+        <v>248.51741939999999</v>
       </c>
       <c r="C15">
-        <v>421.91</v>
+        <v>393.53</v>
       </c>
       <c r="D15">
-        <v>81.8</v>
+        <v>132.19999999999999</v>
       </c>
       <c r="E15">
-        <v>77.3</v>
+        <v>114.6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41639</v>
+        <v>37259</v>
       </c>
       <c r="B16">
-        <v>253.42735479999999</v>
+        <v>202.5226667</v>
       </c>
       <c r="C16">
-        <v>422.01</v>
+        <v>391.75</v>
       </c>
       <c r="D16">
-        <v>90.3</v>
+        <v>114.1</v>
       </c>
       <c r="E16">
-        <v>75.900000000000006</v>
+        <v>113.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41608</v>
+        <v>37315</v>
       </c>
       <c r="B17">
-        <v>266.1829333</v>
+        <v>124.89279999999999</v>
       </c>
       <c r="C17">
-        <v>421.98</v>
+        <v>390.83</v>
       </c>
       <c r="D17">
-        <v>77.599999999999994</v>
+        <v>107.4</v>
       </c>
       <c r="E17">
-        <v>75.3</v>
+        <v>114.6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41578</v>
+        <v>37346</v>
       </c>
       <c r="B18">
-        <v>273.58864519999997</v>
+        <v>155.81866669999999</v>
       </c>
       <c r="C18">
-        <v>421.59</v>
+        <v>389.7</v>
       </c>
       <c r="D18">
-        <v>85.6</v>
+        <v>98.4</v>
       </c>
       <c r="E18">
-        <v>74.900000000000006</v>
+        <v>113.3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41547</v>
+        <v>37376</v>
       </c>
       <c r="B19">
-        <v>281.25279999999998</v>
+        <v>180.86293330000001</v>
       </c>
       <c r="C19">
-        <v>421.79</v>
+        <v>387.62</v>
       </c>
       <c r="D19">
-        <v>37</v>
+        <v>120.7</v>
       </c>
       <c r="E19">
-        <v>73</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41517</v>
+        <v>37389</v>
       </c>
       <c r="B20">
-        <v>269.22890319999999</v>
+        <v>283.02338459999999</v>
       </c>
       <c r="C20">
-        <v>421.99</v>
+        <v>386.64</v>
       </c>
       <c r="D20">
-        <v>66</v>
+        <v>120.8</v>
       </c>
       <c r="E20">
-        <v>68.900000000000006</v>
+        <v>108.8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41486</v>
+        <v>37437</v>
       </c>
       <c r="B21">
-        <v>224.96432429999999</v>
+        <v>248.7542885</v>
       </c>
       <c r="C21">
-        <v>422.21</v>
+        <v>384.12</v>
       </c>
       <c r="D21">
-        <v>57</v>
+        <v>88.3</v>
       </c>
       <c r="E21">
-        <v>65.5</v>
+        <v>106.2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41455</v>
+        <v>37468</v>
       </c>
       <c r="B22">
-        <v>231.18559999999999</v>
+        <v>214.48519229999999</v>
       </c>
       <c r="C22">
-        <v>422.07</v>
+        <v>382.67</v>
       </c>
       <c r="D22">
-        <v>52.5</v>
+        <v>99.6</v>
       </c>
       <c r="E22">
-        <v>62.6</v>
+        <v>102.7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41425</v>
+        <v>37499</v>
       </c>
       <c r="B23">
-        <v>250.23561290000001</v>
+        <v>197.3506442</v>
       </c>
       <c r="C23">
-        <v>421.74</v>
+        <v>380.34</v>
       </c>
       <c r="D23">
-        <v>78.7</v>
+        <v>116.4</v>
       </c>
       <c r="E23">
-        <v>59.9</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41394</v>
+        <v>37529</v>
       </c>
       <c r="B24">
-        <v>255.6112</v>
+        <v>180.21609620000001</v>
       </c>
       <c r="C24">
-        <v>421.59</v>
+        <v>378.96</v>
       </c>
       <c r="D24">
-        <v>72.400000000000006</v>
+        <v>109.6</v>
       </c>
       <c r="E24">
-        <v>57.9</v>
+        <v>94.6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41364</v>
+        <v>37560</v>
       </c>
       <c r="B25">
-        <v>268.28224</v>
+        <v>145.947</v>
       </c>
       <c r="C25">
-        <v>421.85</v>
+        <v>376.99</v>
       </c>
       <c r="D25">
-        <v>57.9</v>
+        <v>97.5</v>
       </c>
       <c r="E25">
-        <v>57.6</v>
+        <v>90.5</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41333</v>
+        <v>37576</v>
       </c>
       <c r="B26">
-        <v>243.18342860000001</v>
+        <v>136.97450000000001</v>
       </c>
       <c r="C26">
-        <v>421.51</v>
+        <v>375.82</v>
       </c>
       <c r="D26">
-        <v>38.1</v>
+        <v>95.5</v>
       </c>
       <c r="E26">
-        <v>58.4</v>
+        <v>85.2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41305</v>
+        <v>37621</v>
       </c>
       <c r="B27">
-        <v>275.33161289999998</v>
+        <v>139.21154110000001</v>
       </c>
       <c r="C27">
-        <v>420.6</v>
+        <v>374.13</v>
       </c>
       <c r="D27">
-        <v>62.9</v>
+        <v>80.8</v>
       </c>
       <c r="E27">
-        <v>58.7</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41274</v>
+        <v>37652</v>
       </c>
       <c r="B28">
-        <v>292.61729029999998</v>
+        <v>141.4485822</v>
       </c>
       <c r="C28">
-        <v>420.46</v>
+        <v>372.25</v>
       </c>
       <c r="D28">
-        <v>40.799999999999997</v>
+        <v>79.7</v>
       </c>
       <c r="E28">
-        <v>59.6</v>
+        <v>80.8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41243</v>
+        <v>37680</v>
       </c>
       <c r="B29">
-        <v>240.05626670000001</v>
+        <v>143.68561349999999</v>
       </c>
       <c r="C29">
-        <v>420.63</v>
+        <v>371.17</v>
       </c>
       <c r="D29">
-        <v>61.8</v>
+        <v>46</v>
       </c>
       <c r="E29">
-        <v>59.7</v>
+        <v>78.3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41213</v>
+        <v>37711</v>
       </c>
       <c r="B30">
-        <v>267.096</v>
+        <v>145.9226645</v>
       </c>
       <c r="C30">
-        <v>420.01</v>
+        <v>370.02</v>
       </c>
       <c r="D30">
-        <v>53.3</v>
+        <v>61.1</v>
       </c>
       <c r="E30">
-        <v>58.6</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41182</v>
+        <v>37741</v>
       </c>
       <c r="B31">
-        <v>310.04382609999999</v>
+        <v>148.1597056</v>
       </c>
       <c r="C31">
-        <v>419.72</v>
+        <v>368.31</v>
       </c>
       <c r="D31">
-        <v>61.4</v>
+        <v>60</v>
       </c>
       <c r="E31">
-        <v>58.1</v>
+        <v>70.099999999999994</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41152</v>
+        <v>37772</v>
       </c>
       <c r="B32">
-        <v>269.58503230000002</v>
+        <v>150.39674669999999</v>
       </c>
       <c r="C32">
-        <v>420.05</v>
+        <v>367.14</v>
       </c>
       <c r="D32">
-        <v>63</v>
+        <v>54.6</v>
       </c>
       <c r="E32">
-        <v>58.2</v>
+        <v>67.599999999999994</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41121</v>
+        <v>37802</v>
       </c>
       <c r="B33">
-        <v>261.18167740000001</v>
+        <v>152.63378779999999</v>
       </c>
       <c r="C33">
-        <v>419.63</v>
+        <v>365.71</v>
       </c>
       <c r="D33">
-        <v>66.5</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="E33">
-        <v>57.8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41090</v>
+        <v>37833</v>
       </c>
       <c r="B34">
-        <v>254.5869333</v>
+        <v>154.87082889999999</v>
       </c>
       <c r="C34">
-        <v>418.64</v>
+        <v>365.16</v>
       </c>
       <c r="D34">
-        <v>64.5</v>
+        <v>83.3</v>
       </c>
       <c r="E34">
-        <v>58.9</v>
+        <v>61.8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41060</v>
+        <v>37864</v>
       </c>
       <c r="B35">
-        <v>240.04464519999999</v>
+        <v>157.10787010000001</v>
       </c>
       <c r="C35">
-        <v>418.56</v>
+        <v>363.56</v>
       </c>
       <c r="D35">
-        <v>69</v>
+        <v>72.7</v>
       </c>
       <c r="E35">
-        <v>61.7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41029</v>
+        <v>37894</v>
       </c>
       <c r="B36">
-        <v>179.54506670000001</v>
+        <v>159.34491120000001</v>
       </c>
       <c r="C36">
-        <v>418.54</v>
+        <v>362.67</v>
       </c>
       <c r="D36">
-        <v>55.2</v>
+        <v>48.7</v>
       </c>
       <c r="E36">
-        <v>64.599999999999994</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>40999</v>
+        <v>37925</v>
       </c>
       <c r="B37">
-        <v>166.12206449999999</v>
+        <v>161.58195230000001</v>
       </c>
       <c r="C37">
-        <v>417.66</v>
+        <v>361.48</v>
       </c>
       <c r="D37">
-        <v>64.3</v>
+        <v>65.5</v>
       </c>
       <c r="E37">
-        <v>66.8</v>
+        <v>58.2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>40968</v>
+        <v>37955</v>
       </c>
       <c r="B38">
-        <v>209.5467586</v>
+        <v>163.81899340000001</v>
       </c>
       <c r="C38">
-        <v>416.38</v>
+        <v>360.33</v>
       </c>
       <c r="D38">
-        <v>32.9</v>
+        <v>67.3</v>
       </c>
       <c r="E38">
-        <v>66.900000000000006</v>
+        <v>56.7</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>40939</v>
+        <v>37986</v>
       </c>
       <c r="B39">
-        <v>214.50425809999999</v>
+        <v>166.05603450000001</v>
       </c>
       <c r="C39">
-        <v>413.62</v>
+        <v>359.58</v>
       </c>
       <c r="D39">
-        <v>58.3</v>
+        <v>46.5</v>
       </c>
       <c r="E39">
-        <v>65.5</v>
+        <v>54.8</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>40908</v>
+        <v>38017</v>
       </c>
       <c r="B40">
-        <v>211.1150968</v>
+        <v>168.2930757</v>
       </c>
       <c r="C40">
-        <v>412.09</v>
+        <v>358.7</v>
       </c>
       <c r="D40">
-        <v>73</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="E40">
-        <v>63.4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>40877</v>
+        <v>38046</v>
       </c>
       <c r="B41">
-        <v>183.05493329999999</v>
+        <v>172.7671579</v>
       </c>
       <c r="C41">
-        <v>410.79</v>
+        <v>357.81</v>
       </c>
       <c r="D41">
-        <v>96.7</v>
+        <v>45.8</v>
       </c>
       <c r="E41">
-        <v>61.1</v>
+        <v>49.3</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>40847</v>
+        <v>38077</v>
       </c>
       <c r="B42">
-        <v>182.58090319999999</v>
+        <v>104.2454194</v>
       </c>
       <c r="C42">
-        <v>409.34</v>
+        <v>356.74</v>
       </c>
       <c r="D42">
-        <v>88</v>
+        <v>49.1</v>
       </c>
       <c r="E42">
-        <v>59.9</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>40816</v>
+        <v>38107</v>
       </c>
       <c r="B43">
-        <v>227.80746669999999</v>
+        <v>92.930133330000004</v>
       </c>
       <c r="C43">
-        <v>407.57</v>
+        <v>355.76</v>
       </c>
       <c r="D43">
-        <v>78</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="E43">
-        <v>59.5</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>40786</v>
+        <v>38138</v>
       </c>
       <c r="B44">
-        <v>249.4923871</v>
+        <v>89.116645160000004</v>
       </c>
       <c r="C44">
-        <v>405.42</v>
+        <v>354.28</v>
       </c>
       <c r="D44">
-        <v>50.6</v>
+        <v>41.5</v>
       </c>
       <c r="E44">
-        <v>59</v>
+        <v>43.8</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>40755</v>
+        <v>38168</v>
       </c>
       <c r="B45">
-        <v>186.35458059999999</v>
+        <v>110.0989333</v>
       </c>
       <c r="C45">
-        <v>404.19</v>
+        <v>354.1</v>
       </c>
       <c r="D45">
-        <v>43.8</v>
+        <v>43.2</v>
       </c>
       <c r="E45">
-        <v>57.3</v>
+        <v>41.6</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>40724</v>
+        <v>38199</v>
       </c>
       <c r="B46">
-        <v>185.66506670000001</v>
+        <v>112.91200000000001</v>
       </c>
       <c r="C46">
-        <v>403.64</v>
+        <v>353.59</v>
       </c>
       <c r="D46">
-        <v>37</v>
+        <v>51.1</v>
       </c>
       <c r="E46">
-        <v>53.2</v>
+        <v>40.200000000000003</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>40694</v>
+        <v>38230</v>
       </c>
       <c r="B47">
-        <v>172.2263226</v>
+        <v>76.085161290000002</v>
       </c>
       <c r="C47">
-        <v>402.2</v>
+        <v>352.83</v>
       </c>
       <c r="D47">
-        <v>41.6</v>
+        <v>40.9</v>
       </c>
       <c r="E47">
-        <v>47.6</v>
+        <v>39.200000000000003</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>40663</v>
+        <v>38260</v>
       </c>
       <c r="B48">
-        <v>176.4261333</v>
+        <v>99.201866670000001</v>
       </c>
       <c r="C48">
-        <v>400.38</v>
+        <v>352.13</v>
       </c>
       <c r="D48">
-        <v>54.4</v>
+        <v>27.7</v>
       </c>
       <c r="E48">
-        <v>41.8</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>40633</v>
+        <v>38291</v>
       </c>
       <c r="B49">
-        <v>42.670709680000002</v>
+        <v>96.810580650000006</v>
       </c>
       <c r="C49">
-        <v>399.48</v>
+        <v>352.02</v>
       </c>
       <c r="D49">
-        <v>55.8</v>
+        <v>48</v>
       </c>
       <c r="E49">
-        <v>36.9</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>40602</v>
+        <v>38321</v>
       </c>
       <c r="B50">
-        <v>154.21342859999999</v>
+        <v>105.55253329999999</v>
       </c>
       <c r="C50">
-        <v>398.44</v>
+        <v>351.15</v>
       </c>
       <c r="D50">
-        <v>29.6</v>
+        <v>43.5</v>
       </c>
       <c r="E50">
-        <v>33.4</v>
+        <v>35.299999999999997</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>40574</v>
+        <v>38352</v>
       </c>
       <c r="B51">
-        <v>147.21393549999999</v>
+        <v>149.29135479999999</v>
       </c>
       <c r="C51">
-        <v>395.89</v>
+        <v>350.93</v>
       </c>
       <c r="D51">
-        <v>18.8</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="E51">
-        <v>30.9</v>
+        <v>35.200000000000003</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>40543</v>
+        <v>38383</v>
       </c>
       <c r="B52">
-        <v>175.00232260000001</v>
+        <v>145.41445160000001</v>
       </c>
       <c r="C52">
-        <v>393.68</v>
+        <v>350.86</v>
       </c>
       <c r="D52">
-        <v>14.4</v>
+        <v>31.3</v>
       </c>
       <c r="E52">
-        <v>28.8</v>
+        <v>34.6</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>40512</v>
+        <v>38411</v>
       </c>
       <c r="B53">
-        <v>195.01653329999999</v>
+        <v>147.9494286</v>
       </c>
       <c r="C53">
-        <v>390.7</v>
+        <v>349.84</v>
       </c>
       <c r="D53">
-        <v>21.5</v>
+        <v>29.2</v>
       </c>
       <c r="E53">
-        <v>26.5</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>40482</v>
+        <v>38442</v>
       </c>
       <c r="B54">
-        <v>219.1210323</v>
+        <v>177.60593549999999</v>
       </c>
       <c r="C54">
-        <v>388.64</v>
+        <v>350.33</v>
       </c>
       <c r="D54">
-        <v>23.5</v>
+        <v>24.5</v>
       </c>
       <c r="E54">
-        <v>23.2</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>40451</v>
+        <v>38472</v>
       </c>
       <c r="B55">
-        <v>170.22266669999999</v>
+        <v>143.0965333</v>
       </c>
       <c r="C55">
-        <v>386.54</v>
+        <v>350.25</v>
       </c>
       <c r="D55">
-        <v>25.2</v>
+        <v>24.2</v>
       </c>
       <c r="E55">
-        <v>19.600000000000001</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>40421</v>
+        <v>38503</v>
       </c>
       <c r="B56">
-        <v>219.50916129999999</v>
+        <v>133.6188387</v>
       </c>
       <c r="C56">
-        <v>379.98</v>
+        <v>349.23</v>
       </c>
       <c r="D56">
-        <v>19.600000000000001</v>
+        <v>42.7</v>
       </c>
       <c r="E56">
-        <v>17.399999999999999</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>40390</v>
+        <v>38533</v>
       </c>
       <c r="B57">
-        <v>232.55741939999999</v>
+        <v>124.75973329999999</v>
       </c>
       <c r="C57">
-        <v>374.94</v>
+        <v>348.3</v>
       </c>
       <c r="D57">
-        <v>16.100000000000001</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="E57">
-        <v>16.7</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>40359</v>
+        <v>38564</v>
       </c>
       <c r="B58">
-        <v>156.876</v>
+        <v>87.702967740000005</v>
       </c>
       <c r="C58">
-        <v>372.88</v>
+        <v>348.47</v>
       </c>
       <c r="D58">
-        <v>13.6</v>
+        <v>40.1</v>
       </c>
       <c r="E58">
-        <v>16.399999999999999</v>
+        <v>29.1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>40329</v>
+        <v>38595</v>
       </c>
       <c r="B59">
-        <v>188.56645159999999</v>
+        <v>135.09470970000001</v>
       </c>
       <c r="C59">
-        <v>371.33</v>
+        <v>348</v>
       </c>
       <c r="D59">
-        <v>8.6999999999999993</v>
+        <v>36.4</v>
       </c>
       <c r="E59">
-        <v>15.5</v>
+        <v>27.4</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>40298</v>
+        <v>38625</v>
       </c>
       <c r="B60">
-        <v>201.92026670000001</v>
+        <v>85.927733329999995</v>
       </c>
       <c r="C60">
-        <v>369.54</v>
+        <v>347.26</v>
       </c>
       <c r="D60">
-        <v>8</v>
+        <v>21.9</v>
       </c>
       <c r="E60">
-        <v>14</v>
+        <v>25.8</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>40268</v>
+        <v>38656</v>
       </c>
       <c r="B61">
-        <v>259.84335479999999</v>
+        <v>134.60645160000001</v>
       </c>
       <c r="C61">
-        <v>367.87</v>
+        <v>347.54</v>
       </c>
       <c r="D61">
-        <v>15.4</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E61">
-        <v>12.3</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>40237</v>
+        <v>38686</v>
       </c>
       <c r="B62">
-        <v>182.09114289999999</v>
+        <v>120.5528</v>
       </c>
       <c r="C62">
-        <v>366.16</v>
+        <v>347.9</v>
       </c>
       <c r="D62">
-        <v>18.8</v>
+        <v>18</v>
       </c>
       <c r="E62">
-        <v>10.6</v>
+        <v>24.9</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>40209</v>
+        <v>38717</v>
       </c>
       <c r="B63">
-        <v>202.9220645</v>
+        <v>100.57367739999999</v>
       </c>
       <c r="C63">
-        <v>365.14</v>
+        <v>347.46</v>
       </c>
       <c r="D63">
-        <v>13.2</v>
+        <v>41.1</v>
       </c>
       <c r="E63">
-        <v>9.3000000000000007</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>40178</v>
+        <v>38748</v>
       </c>
       <c r="B64">
-        <v>200.4972903</v>
+        <v>104.7615484</v>
       </c>
       <c r="C64">
-        <v>363.88</v>
+        <v>348.14</v>
       </c>
       <c r="D64">
-        <v>10.8</v>
+        <v>15.3</v>
       </c>
       <c r="E64">
-        <v>8.3000000000000007</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>40147</v>
+        <v>38776</v>
       </c>
       <c r="B65">
-        <v>202.9397333</v>
+        <v>96.685142859999999</v>
       </c>
       <c r="C65">
-        <v>362.59</v>
+        <v>348.29</v>
       </c>
       <c r="D65">
-        <v>4.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E65">
-        <v>7.6</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>40117</v>
+        <v>38807</v>
       </c>
       <c r="B66">
-        <v>161.21419349999999</v>
+        <v>77.60954839</v>
       </c>
       <c r="C66">
-        <v>362.24</v>
+        <v>348.39</v>
       </c>
       <c r="D66">
-        <v>4.8</v>
+        <v>10.6</v>
       </c>
       <c r="E66">
-        <v>7.1</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>40086</v>
+        <v>38837</v>
       </c>
       <c r="B67">
-        <v>188.47093330000001</v>
+        <v>96.942133330000004</v>
       </c>
       <c r="C67">
-        <v>361.51</v>
+        <v>348.5</v>
       </c>
       <c r="D67">
-        <v>4.3</v>
+        <v>30.2</v>
       </c>
       <c r="E67">
-        <v>6.2</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>40056</v>
+        <v>38868</v>
       </c>
       <c r="B68">
-        <v>233.1445161</v>
+        <v>90.061935480000002</v>
       </c>
       <c r="C68">
-        <v>360.67</v>
+        <v>348.39</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>22.3</v>
       </c>
       <c r="E68">
-        <v>4.8</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>40025</v>
+        <v>38898</v>
       </c>
       <c r="B69">
-        <v>236.38529030000001</v>
+        <v>84.2072</v>
       </c>
       <c r="C69">
-        <v>359.48</v>
+        <v>349.07</v>
       </c>
       <c r="D69">
-        <v>3.2</v>
+        <v>13.9</v>
       </c>
       <c r="E69">
-        <v>3.6</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>39994</v>
+        <v>38929</v>
       </c>
       <c r="B70">
-        <v>240.47866669999999</v>
+        <v>80.470193550000005</v>
       </c>
       <c r="C70">
-        <v>358.79</v>
+        <v>349.74</v>
       </c>
       <c r="D70">
-        <v>2.9</v>
+        <v>12.2</v>
       </c>
       <c r="E70">
-        <v>2.7</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>39964</v>
+        <v>38960</v>
       </c>
       <c r="B71">
-        <v>236.4449032</v>
+        <v>0.43612903200000003</v>
       </c>
       <c r="C71">
-        <v>358.23</v>
+        <v>350.01</v>
       </c>
       <c r="D71">
-        <v>2.9</v>
+        <v>12.9</v>
       </c>
       <c r="E71">
-        <v>2.2999999999999998</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>39933</v>
+        <v>38978</v>
       </c>
       <c r="B72">
-        <v>206.9266667</v>
+        <v>3.6444443999999999E-2</v>
       </c>
       <c r="C72">
-        <v>357.29</v>
+        <v>350.99</v>
       </c>
       <c r="D72">
-        <v>0.8</v>
+        <v>14.4</v>
       </c>
       <c r="E72">
-        <v>2.2000000000000002</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>39903</v>
+        <v>39021</v>
       </c>
       <c r="B73">
-        <v>202.2167742</v>
+        <v>20.9096385</v>
       </c>
       <c r="C73">
-        <v>356.13</v>
+        <v>351.04</v>
       </c>
       <c r="D73">
-        <v>0.7</v>
+        <v>10.5</v>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>39872</v>
+        <v>39051</v>
       </c>
       <c r="B74">
-        <v>176.56942860000001</v>
+        <v>41.782832999999997</v>
       </c>
       <c r="C74">
-        <v>355.42</v>
+        <v>351.85</v>
       </c>
       <c r="D74">
-        <v>1.4</v>
+        <v>21.4</v>
       </c>
       <c r="E74">
-        <v>1.9</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>39844</v>
+        <v>39082</v>
       </c>
       <c r="B75">
-        <v>216.70451610000001</v>
+        <v>62.656016649999998</v>
       </c>
       <c r="C75">
-        <v>354.76</v>
+        <v>353.06</v>
       </c>
       <c r="D75">
-        <v>1.3</v>
+        <v>13.6</v>
       </c>
       <c r="E75">
-        <v>1.8</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>39813</v>
+        <v>39113</v>
       </c>
       <c r="B76">
-        <v>189.5793548</v>
+        <v>83.529200000000003</v>
       </c>
       <c r="C76">
-        <v>354.75</v>
+        <v>354.51</v>
       </c>
       <c r="D76">
-        <v>0.8</v>
+        <v>16.8</v>
       </c>
       <c r="E76">
-        <v>1.7</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>39782</v>
+        <v>39172</v>
       </c>
       <c r="B77">
-        <v>165.9362667</v>
+        <v>104.20399999999999</v>
       </c>
       <c r="C77">
-        <v>354.73</v>
+        <v>355.15</v>
       </c>
       <c r="D77">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="E77">
-        <v>1.7</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>39752</v>
+        <v>39202</v>
       </c>
       <c r="B78">
-        <v>161.82425810000001</v>
+        <v>125.2756</v>
       </c>
       <c r="C78">
-        <v>353.94</v>
+        <v>355.42</v>
       </c>
       <c r="D78">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="E78">
-        <v>1.8</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>39721</v>
+        <v>39233</v>
       </c>
       <c r="B79">
-        <v>272.16586669999998</v>
+        <v>146.14879999999999</v>
       </c>
       <c r="C79">
-        <v>353.49</v>
+        <v>356.38</v>
       </c>
       <c r="D79">
-        <v>1.1000000000000001</v>
+        <v>11.7</v>
       </c>
       <c r="E79">
-        <v>2.2999999999999998</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>39691</v>
+        <v>39263</v>
       </c>
       <c r="B80">
-        <v>246.46709680000001</v>
+        <v>167.02199999999999</v>
       </c>
       <c r="C80">
-        <v>353.89</v>
+        <v>356.62</v>
       </c>
       <c r="D80">
-        <v>0.5</v>
+        <v>12.1</v>
       </c>
       <c r="E80">
-        <v>2.7</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>39660</v>
+        <v>39294</v>
       </c>
       <c r="B81">
-        <v>151.13703229999999</v>
+        <v>138.4745806</v>
       </c>
       <c r="C81">
-        <v>354.11</v>
+        <v>356.73</v>
       </c>
       <c r="D81">
-        <v>0.8</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="E81">
-        <v>2.8</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>39629</v>
+        <v>39325</v>
       </c>
       <c r="B82">
-        <v>178.82270969999999</v>
+        <v>145.6420645</v>
       </c>
       <c r="C82">
-        <v>354.47</v>
+        <v>357.17</v>
       </c>
       <c r="D82">
-        <v>3.4</v>
+        <v>6</v>
       </c>
       <c r="E82">
-        <v>3.3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>39599</v>
+        <v>39355</v>
       </c>
       <c r="B83">
-        <v>186.3956129</v>
+        <v>184.92826669999999</v>
       </c>
       <c r="C83">
-        <v>355.13</v>
+        <v>357.23</v>
       </c>
       <c r="D83">
-        <v>3.2</v>
+        <v>2.4</v>
       </c>
       <c r="E83">
-        <v>3.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>39568</v>
+        <v>39386</v>
       </c>
       <c r="B84">
-        <v>140.0357333</v>
+        <v>185.95509680000001</v>
       </c>
       <c r="C84">
-        <v>355.35</v>
+        <v>356.87</v>
       </c>
       <c r="D84">
-        <v>2.9</v>
+        <v>0.9</v>
       </c>
       <c r="E84">
-        <v>3.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>39538</v>
+        <v>39416</v>
       </c>
       <c r="B85">
-        <v>204.52799999999999</v>
+        <v>186.89279999999999</v>
       </c>
       <c r="C85">
-        <v>355.03</v>
+        <v>356.01</v>
       </c>
       <c r="D85">
-        <v>9.3000000000000007</v>
+        <v>1.7</v>
       </c>
       <c r="E85">
-        <v>3.3</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>39507</v>
+        <v>39447</v>
       </c>
       <c r="B86">
-        <v>167.94151719999999</v>
+        <v>192.4787097</v>
       </c>
       <c r="C86">
-        <v>355.57</v>
+        <v>356.34</v>
       </c>
       <c r="D86">
-        <v>2.1</v>
+        <v>10.1</v>
       </c>
       <c r="E86">
-        <v>3.6</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2336,1450 +2334,1453 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>39447</v>
+        <v>39507</v>
       </c>
       <c r="B88">
-        <v>192.4787097</v>
+        <v>167.94151719999999</v>
       </c>
       <c r="C88">
-        <v>356.34</v>
+        <v>355.57</v>
       </c>
       <c r="D88">
-        <v>10.1</v>
+        <v>2.1</v>
       </c>
       <c r="E88">
-        <v>4.9000000000000004</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>39416</v>
+        <v>39538</v>
       </c>
       <c r="B89">
-        <v>186.89279999999999</v>
+        <v>204.52799999999999</v>
       </c>
       <c r="C89">
-        <v>356.01</v>
+        <v>355.03</v>
       </c>
       <c r="D89">
-        <v>1.7</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E89">
-        <v>5.7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>39386</v>
+        <v>39568</v>
       </c>
       <c r="B90">
-        <v>185.95509680000001</v>
+        <v>140.0357333</v>
       </c>
       <c r="C90">
-        <v>356.87</v>
+        <v>355.35</v>
       </c>
       <c r="D90">
-        <v>0.9</v>
+        <v>2.9</v>
       </c>
       <c r="E90">
-        <v>6</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>39355</v>
+        <v>39599</v>
       </c>
       <c r="B91">
-        <v>184.92826669999999</v>
+        <v>186.3956129</v>
       </c>
       <c r="C91">
-        <v>357.23</v>
+        <v>355.13</v>
       </c>
       <c r="D91">
-        <v>2.4</v>
+        <v>3.2</v>
       </c>
       <c r="E91">
-        <v>5.9</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>39325</v>
+        <v>39629</v>
       </c>
       <c r="B92">
-        <v>145.6420645</v>
+        <v>178.82270969999999</v>
       </c>
       <c r="C92">
-        <v>357.17</v>
+        <v>354.47</v>
       </c>
       <c r="D92">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="E92">
-        <v>6</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>39294</v>
+        <v>39660</v>
       </c>
       <c r="B93">
-        <v>138.4745806</v>
+        <v>151.13703229999999</v>
       </c>
       <c r="C93">
-        <v>356.73</v>
+        <v>354.11</v>
       </c>
       <c r="D93">
-        <v>9.6999999999999993</v>
+        <v>0.8</v>
       </c>
       <c r="E93">
-        <v>6.9</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>39263</v>
+        <v>39691</v>
       </c>
       <c r="B94">
-        <v>167.02199999999999</v>
+        <v>246.46709680000001</v>
       </c>
       <c r="C94">
-        <v>356.62</v>
+        <v>353.89</v>
       </c>
       <c r="D94">
-        <v>12.1</v>
+        <v>0.5</v>
       </c>
       <c r="E94">
-        <v>7.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>39233</v>
+        <v>39721</v>
       </c>
       <c r="B95">
-        <v>146.14879999999999</v>
+        <v>272.16586669999998</v>
       </c>
       <c r="C95">
-        <v>356.38</v>
+        <v>353.49</v>
       </c>
       <c r="D95">
-        <v>11.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E95">
-        <v>8.6</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>39202</v>
+        <v>39752</v>
       </c>
       <c r="B96">
-        <v>125.2756</v>
+        <v>161.82425810000001</v>
       </c>
       <c r="C96">
-        <v>355.42</v>
+        <v>353.94</v>
       </c>
       <c r="D96">
-        <v>3.4</v>
+        <v>2.9</v>
       </c>
       <c r="E96">
-        <v>9.8000000000000007</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>39172</v>
+        <v>39782</v>
       </c>
       <c r="B97">
-        <v>104.20399999999999</v>
+        <v>165.9362667</v>
       </c>
       <c r="C97">
-        <v>355.15</v>
+        <v>354.73</v>
       </c>
       <c r="D97">
-        <v>4.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E97">
-        <v>10.7</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>39113</v>
+        <v>39813</v>
       </c>
       <c r="B98">
-        <v>83.529200000000003</v>
+        <v>189.5793548</v>
       </c>
       <c r="C98">
-        <v>354.51</v>
+        <v>354.75</v>
       </c>
       <c r="D98">
-        <v>16.8</v>
+        <v>0.8</v>
       </c>
       <c r="E98">
-        <v>11.9</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>39082</v>
+        <v>39844</v>
       </c>
       <c r="B99">
-        <v>62.656016649999998</v>
+        <v>216.70451610000001</v>
       </c>
       <c r="C99">
-        <v>353.06</v>
+        <v>354.76</v>
       </c>
       <c r="D99">
-        <v>13.6</v>
+        <v>1.3</v>
       </c>
       <c r="E99">
-        <v>12.1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>39051</v>
+        <v>39872</v>
       </c>
       <c r="B100">
-        <v>41.782832999999997</v>
+        <v>176.56942860000001</v>
       </c>
       <c r="C100">
-        <v>351.85</v>
+        <v>355.42</v>
       </c>
       <c r="D100">
-        <v>21.4</v>
+        <v>1.4</v>
       </c>
       <c r="E100">
-        <v>12.6</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>39021</v>
+        <v>39903</v>
       </c>
       <c r="B101">
-        <v>20.9096385</v>
+        <v>202.2167742</v>
       </c>
       <c r="C101">
-        <v>351.04</v>
+        <v>356.13</v>
       </c>
       <c r="D101">
-        <v>10.5</v>
+        <v>0.7</v>
       </c>
       <c r="E101">
-        <v>14.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>38978</v>
+        <v>39933</v>
       </c>
       <c r="B102">
-        <v>3.6444443999999999E-2</v>
+        <v>206.9266667</v>
       </c>
       <c r="C102">
-        <v>350.99</v>
+        <v>357.29</v>
       </c>
       <c r="D102">
-        <v>14.4</v>
+        <v>0.8</v>
       </c>
       <c r="E102">
-        <v>15.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>38960</v>
+        <v>39964</v>
       </c>
       <c r="B103">
-        <v>0.43612903200000003</v>
+        <v>236.4449032</v>
       </c>
       <c r="C103">
-        <v>350.01</v>
+        <v>358.23</v>
       </c>
       <c r="D103">
-        <v>12.9</v>
+        <v>2.9</v>
       </c>
       <c r="E103">
-        <v>15.6</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>38929</v>
+        <v>39994</v>
       </c>
       <c r="B104">
-        <v>80.470193550000005</v>
+        <v>240.47866669999999</v>
       </c>
       <c r="C104">
-        <v>349.74</v>
+        <v>358.79</v>
       </c>
       <c r="D104">
-        <v>12.2</v>
+        <v>2.9</v>
       </c>
       <c r="E104">
-        <v>15.2</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>38898</v>
+        <v>40025</v>
       </c>
       <c r="B105">
-        <v>84.2072</v>
+        <v>236.38529030000001</v>
       </c>
       <c r="C105">
-        <v>349.07</v>
+        <v>359.48</v>
       </c>
       <c r="D105">
-        <v>13.9</v>
+        <v>3.2</v>
       </c>
       <c r="E105">
-        <v>16.3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>38868</v>
+        <v>40056</v>
       </c>
       <c r="B106">
-        <v>90.061935480000002</v>
+        <v>233.1445161</v>
       </c>
       <c r="C106">
-        <v>348.39</v>
+        <v>360.67</v>
       </c>
       <c r="D106">
-        <v>22.3</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>17.3</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>38837</v>
+        <v>40086</v>
       </c>
       <c r="B107">
-        <v>96.942133330000004</v>
+        <v>188.47093330000001</v>
       </c>
       <c r="C107">
-        <v>348.5</v>
+        <v>361.51</v>
       </c>
       <c r="D107">
-        <v>30.2</v>
+        <v>4.3</v>
       </c>
       <c r="E107">
-        <v>17.100000000000001</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>38807</v>
+        <v>40117</v>
       </c>
       <c r="B108">
-        <v>77.60954839</v>
+        <v>161.21419349999999</v>
       </c>
       <c r="C108">
-        <v>348.39</v>
+        <v>362.24</v>
       </c>
       <c r="D108">
-        <v>10.6</v>
+        <v>4.8</v>
       </c>
       <c r="E108">
-        <v>17.399999999999999</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>38776</v>
+        <v>40147</v>
       </c>
       <c r="B109">
-        <v>96.685142859999999</v>
+        <v>202.9397333</v>
       </c>
       <c r="C109">
-        <v>348.29</v>
+        <v>362.59</v>
       </c>
       <c r="D109">
-        <v>4.9000000000000004</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E109">
-        <v>18.600000000000001</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>38748</v>
+        <v>40178</v>
       </c>
       <c r="B110">
-        <v>104.7615484</v>
+        <v>200.4972903</v>
       </c>
       <c r="C110">
-        <v>348.14</v>
+        <v>363.88</v>
       </c>
       <c r="D110">
-        <v>15.3</v>
+        <v>10.8</v>
       </c>
       <c r="E110">
-        <v>20.8</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>38717</v>
+        <v>40209</v>
       </c>
       <c r="B111">
-        <v>100.57367739999999</v>
+        <v>202.9220645</v>
       </c>
       <c r="C111">
-        <v>347.46</v>
+        <v>365.14</v>
       </c>
       <c r="D111">
-        <v>41.1</v>
+        <v>13.2</v>
       </c>
       <c r="E111">
-        <v>23</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>38686</v>
+        <v>40237</v>
       </c>
       <c r="B112">
-        <v>120.5528</v>
+        <v>182.09114289999999</v>
       </c>
       <c r="C112">
-        <v>347.9</v>
+        <v>366.16</v>
       </c>
       <c r="D112">
-        <v>18</v>
+        <v>18.8</v>
       </c>
       <c r="E112">
-        <v>24.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>38656</v>
+        <v>40268</v>
       </c>
       <c r="B113">
-        <v>134.60645160000001</v>
+        <v>259.84335479999999</v>
       </c>
       <c r="C113">
-        <v>347.54</v>
+        <v>367.87</v>
       </c>
       <c r="D113">
-        <v>8.6999999999999993</v>
+        <v>15.4</v>
       </c>
       <c r="E113">
-        <v>25.5</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>38625</v>
+        <v>40298</v>
       </c>
       <c r="B114">
-        <v>85.927733329999995</v>
+        <v>201.92026670000001</v>
       </c>
       <c r="C114">
-        <v>347.26</v>
+        <v>369.54</v>
       </c>
       <c r="D114">
-        <v>21.9</v>
+        <v>8</v>
       </c>
       <c r="E114">
-        <v>25.8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>38595</v>
+        <v>40329</v>
       </c>
       <c r="B115">
-        <v>135.09470970000001</v>
+        <v>188.56645159999999</v>
       </c>
       <c r="C115">
-        <v>348</v>
+        <v>371.33</v>
       </c>
       <c r="D115">
-        <v>36.4</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E115">
-        <v>27.4</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>38564</v>
+        <v>40359</v>
       </c>
       <c r="B116">
-        <v>87.702967740000005</v>
+        <v>156.876</v>
       </c>
       <c r="C116">
-        <v>348.47</v>
+        <v>372.88</v>
       </c>
       <c r="D116">
-        <v>40.1</v>
+        <v>13.6</v>
       </c>
       <c r="E116">
-        <v>29.1</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>38533</v>
+        <v>40390</v>
       </c>
       <c r="B117">
-        <v>124.75973329999999</v>
+        <v>232.55741939999999</v>
       </c>
       <c r="C117">
-        <v>348.3</v>
+        <v>374.94</v>
       </c>
       <c r="D117">
-        <v>39.299999999999997</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="E117">
-        <v>28.8</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>38503</v>
+        <v>40421</v>
       </c>
       <c r="B118">
-        <v>133.6188387</v>
+        <v>219.50916129999999</v>
       </c>
       <c r="C118">
-        <v>349.23</v>
+        <v>379.98</v>
       </c>
       <c r="D118">
-        <v>42.7</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E118">
-        <v>28.9</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>38472</v>
+        <v>40451</v>
       </c>
       <c r="B119">
-        <v>143.0965333</v>
+        <v>170.22266669999999</v>
       </c>
       <c r="C119">
-        <v>350.25</v>
+        <v>386.54</v>
       </c>
       <c r="D119">
-        <v>24.2</v>
+        <v>25.2</v>
       </c>
       <c r="E119">
-        <v>31.6</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>38442</v>
+        <v>40482</v>
       </c>
       <c r="B120">
-        <v>177.60593549999999</v>
+        <v>219.1210323</v>
       </c>
       <c r="C120">
-        <v>350.33</v>
+        <v>388.64</v>
       </c>
       <c r="D120">
-        <v>24.5</v>
+        <v>23.5</v>
       </c>
       <c r="E120">
-        <v>33.5</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>38411</v>
+        <v>40512</v>
       </c>
       <c r="B121">
-        <v>147.9494286</v>
+        <v>195.01653329999999</v>
       </c>
       <c r="C121">
-        <v>349.84</v>
+        <v>390.7</v>
       </c>
       <c r="D121">
-        <v>29.2</v>
+        <v>21.5</v>
       </c>
       <c r="E121">
-        <v>33.9</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>38383</v>
+        <v>40543</v>
       </c>
       <c r="B122">
-        <v>145.41445160000001</v>
+        <v>175.00232260000001</v>
       </c>
       <c r="C122">
-        <v>350.86</v>
+        <v>393.68</v>
       </c>
       <c r="D122">
-        <v>31.3</v>
+        <v>14.4</v>
       </c>
       <c r="E122">
-        <v>34.6</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>38352</v>
+        <v>40574</v>
       </c>
       <c r="B123">
-        <v>149.29135479999999</v>
+        <v>147.21393549999999</v>
       </c>
       <c r="C123">
-        <v>350.93</v>
+        <v>395.89</v>
       </c>
       <c r="D123">
-        <v>17.899999999999999</v>
+        <v>18.8</v>
       </c>
       <c r="E123">
-        <v>35.200000000000003</v>
+        <v>30.9</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>38321</v>
+        <v>40602</v>
       </c>
       <c r="B124">
-        <v>105.55253329999999</v>
+        <v>154.21342859999999</v>
       </c>
       <c r="C124">
-        <v>351.15</v>
+        <v>398.44</v>
       </c>
       <c r="D124">
-        <v>43.5</v>
+        <v>29.6</v>
       </c>
       <c r="E124">
-        <v>35.299999999999997</v>
+        <v>33.4</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>38291</v>
+        <v>40633</v>
       </c>
       <c r="B125">
-        <v>96.810580650000006</v>
+        <v>42.670709680000002</v>
       </c>
       <c r="C125">
-        <v>352.02</v>
+        <v>399.48</v>
       </c>
       <c r="D125">
-        <v>48</v>
+        <v>55.8</v>
       </c>
       <c r="E125">
-        <v>35.9</v>
+        <v>36.9</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>38260</v>
+        <v>40663</v>
       </c>
       <c r="B126">
-        <v>99.201866670000001</v>
+        <v>176.4261333</v>
       </c>
       <c r="C126">
-        <v>352.13</v>
+        <v>400.38</v>
       </c>
       <c r="D126">
-        <v>27.7</v>
+        <v>54.4</v>
       </c>
       <c r="E126">
-        <v>37.5</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>38230</v>
+        <v>40694</v>
       </c>
       <c r="B127">
-        <v>76.085161290000002</v>
+        <v>172.2263226</v>
       </c>
       <c r="C127">
-        <v>352.83</v>
+        <v>402.2</v>
       </c>
       <c r="D127">
-        <v>40.9</v>
+        <v>41.6</v>
       </c>
       <c r="E127">
-        <v>39.200000000000003</v>
+        <v>47.6</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>38199</v>
+        <v>40724</v>
       </c>
       <c r="B128">
-        <v>112.91200000000001</v>
+        <v>185.66506670000001</v>
       </c>
       <c r="C128">
-        <v>353.59</v>
+        <v>403.64</v>
       </c>
       <c r="D128">
-        <v>51.1</v>
+        <v>37</v>
       </c>
       <c r="E128">
-        <v>40.200000000000003</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>38168</v>
+        <v>40755</v>
       </c>
       <c r="B129">
-        <v>110.0989333</v>
+        <v>186.35458059999999</v>
       </c>
       <c r="C129">
-        <v>354.1</v>
+        <v>404.19</v>
       </c>
       <c r="D129">
-        <v>43.2</v>
+        <v>43.8</v>
       </c>
       <c r="E129">
-        <v>41.6</v>
+        <v>57.3</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>38138</v>
+        <v>40786</v>
       </c>
       <c r="B130">
-        <v>89.116645160000004</v>
+        <v>249.4923871</v>
       </c>
       <c r="C130">
-        <v>354.28</v>
+        <v>405.42</v>
       </c>
       <c r="D130">
-        <v>41.5</v>
+        <v>50.6</v>
       </c>
       <c r="E130">
-        <v>43.8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>38107</v>
+        <v>40816</v>
       </c>
       <c r="B131">
-        <v>92.930133330000004</v>
+        <v>227.80746669999999</v>
       </c>
       <c r="C131">
-        <v>355.76</v>
+        <v>407.57</v>
       </c>
       <c r="D131">
-        <v>39.299999999999997</v>
+        <v>78</v>
       </c>
       <c r="E131">
-        <v>45.5</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>38077</v>
+        <v>40847</v>
       </c>
       <c r="B132">
-        <v>104.2454194</v>
+        <v>182.58090319999999</v>
       </c>
       <c r="C132">
-        <v>356.74</v>
+        <v>409.34</v>
       </c>
       <c r="D132">
-        <v>49.1</v>
+        <v>88</v>
       </c>
       <c r="E132">
-        <v>47.1</v>
+        <v>59.9</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>38046</v>
+        <v>40877</v>
       </c>
       <c r="B133">
-        <v>172.7671579</v>
+        <v>183.05493329999999</v>
       </c>
       <c r="C133">
-        <v>357.81</v>
+        <v>410.79</v>
       </c>
       <c r="D133">
-        <v>45.8</v>
+        <v>96.7</v>
       </c>
       <c r="E133">
-        <v>49.3</v>
+        <v>61.1</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>38017</v>
+        <v>40908</v>
       </c>
       <c r="B134">
-        <v>168.2930757</v>
+        <v>211.1150968</v>
       </c>
       <c r="C134">
-        <v>358.7</v>
+        <v>412.09</v>
       </c>
       <c r="D134">
-        <v>37.299999999999997</v>
+        <v>73</v>
       </c>
       <c r="E134">
-        <v>52</v>
+        <v>63.4</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>37986</v>
+        <v>40939</v>
       </c>
       <c r="B135">
-        <v>166.05603450000001</v>
+        <v>214.50425809999999</v>
       </c>
       <c r="C135">
-        <v>359.58</v>
+        <v>413.62</v>
       </c>
       <c r="D135">
-        <v>46.5</v>
+        <v>58.3</v>
       </c>
       <c r="E135">
-        <v>54.8</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>37955</v>
+        <v>40968</v>
       </c>
       <c r="B136">
-        <v>163.81899340000001</v>
+        <v>209.5467586</v>
       </c>
       <c r="C136">
-        <v>360.33</v>
+        <v>416.38</v>
       </c>
       <c r="D136">
-        <v>67.3</v>
+        <v>32.9</v>
       </c>
       <c r="E136">
-        <v>56.7</v>
+        <v>66.900000000000006</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>37925</v>
+        <v>40999</v>
       </c>
       <c r="B137">
-        <v>161.58195230000001</v>
+        <v>166.12206449999999</v>
       </c>
       <c r="C137">
-        <v>361.48</v>
+        <v>417.66</v>
       </c>
       <c r="D137">
-        <v>65.5</v>
+        <v>64.3</v>
       </c>
       <c r="E137">
-        <v>58.2</v>
+        <v>66.8</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>37894</v>
+        <v>41029</v>
       </c>
       <c r="B138">
-        <v>159.34491120000001</v>
+        <v>179.54506670000001</v>
       </c>
       <c r="C138">
-        <v>362.67</v>
+        <v>418.54</v>
       </c>
       <c r="D138">
-        <v>48.7</v>
+        <v>55.2</v>
       </c>
       <c r="E138">
-        <v>59.5</v>
+        <v>64.599999999999994</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>37864</v>
+        <v>41060</v>
       </c>
       <c r="B139">
-        <v>157.10787010000001</v>
+        <v>240.04464519999999</v>
       </c>
       <c r="C139">
-        <v>363.56</v>
+        <v>418.56</v>
       </c>
       <c r="D139">
-        <v>72.7</v>
+        <v>69</v>
       </c>
       <c r="E139">
-        <v>60</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>37833</v>
+        <v>41090</v>
       </c>
       <c r="B140">
-        <v>154.87082889999999</v>
+        <v>254.5869333</v>
       </c>
       <c r="C140">
-        <v>365.16</v>
+        <v>418.64</v>
       </c>
       <c r="D140">
-        <v>83.3</v>
+        <v>64.5</v>
       </c>
       <c r="E140">
-        <v>61.8</v>
+        <v>58.9</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>37802</v>
+        <v>41121</v>
       </c>
       <c r="B141">
-        <v>152.63378779999999</v>
+        <v>261.18167740000001</v>
       </c>
       <c r="C141">
-        <v>365.71</v>
+        <v>419.63</v>
       </c>
       <c r="D141">
-        <v>77.400000000000006</v>
+        <v>66.5</v>
       </c>
       <c r="E141">
-        <v>65</v>
+        <v>57.8</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>37772</v>
+        <v>41152</v>
       </c>
       <c r="B142">
-        <v>150.39674669999999</v>
+        <v>269.58503230000002</v>
       </c>
       <c r="C142">
-        <v>367.14</v>
+        <v>420.05</v>
       </c>
       <c r="D142">
-        <v>54.6</v>
+        <v>63</v>
       </c>
       <c r="E142">
-        <v>67.599999999999994</v>
+        <v>58.2</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>37741</v>
+        <v>41182</v>
       </c>
       <c r="B143">
-        <v>148.1597056</v>
+        <v>310.04382609999999</v>
       </c>
       <c r="C143">
-        <v>368.31</v>
+        <v>419.72</v>
       </c>
       <c r="D143">
-        <v>60</v>
+        <v>61.4</v>
       </c>
       <c r="E143">
-        <v>70.099999999999994</v>
+        <v>58.1</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>37711</v>
+        <v>41213</v>
       </c>
       <c r="B144">
-        <v>145.9226645</v>
+        <v>267.096</v>
       </c>
       <c r="C144">
-        <v>370.02</v>
+        <v>420.01</v>
       </c>
       <c r="D144">
-        <v>61.1</v>
+        <v>53.3</v>
       </c>
       <c r="E144">
-        <v>74</v>
+        <v>58.6</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>37680</v>
+        <v>41243</v>
       </c>
       <c r="B145">
-        <v>143.68561349999999</v>
+        <v>240.05626670000001</v>
       </c>
       <c r="C145">
-        <v>371.17</v>
+        <v>420.63</v>
       </c>
       <c r="D145">
-        <v>46</v>
+        <v>61.8</v>
       </c>
       <c r="E145">
-        <v>78.3</v>
+        <v>59.7</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>37652</v>
+        <v>41274</v>
       </c>
       <c r="B146">
-        <v>141.4485822</v>
+        <v>292.61729029999998</v>
       </c>
       <c r="C146">
-        <v>372.25</v>
+        <v>420.46</v>
       </c>
       <c r="D146">
-        <v>79.7</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="E146">
-        <v>80.8</v>
+        <v>59.6</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>37621</v>
+        <v>41305</v>
       </c>
       <c r="B147">
-        <v>139.21154110000001</v>
+        <v>275.33161289999998</v>
       </c>
       <c r="C147">
-        <v>374.13</v>
+        <v>420.6</v>
       </c>
       <c r="D147">
-        <v>80.8</v>
+        <v>62.9</v>
       </c>
       <c r="E147">
-        <v>82</v>
+        <v>58.7</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>37576</v>
+        <v>41333</v>
       </c>
       <c r="B148">
-        <v>136.97450000000001</v>
+        <v>243.18342860000001</v>
       </c>
       <c r="C148">
-        <v>375.82</v>
+        <v>421.51</v>
       </c>
       <c r="D148">
-        <v>95.5</v>
+        <v>38.1</v>
       </c>
       <c r="E148">
-        <v>85.2</v>
+        <v>58.4</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>37560</v>
+        <v>41364</v>
       </c>
       <c r="B149">
-        <v>145.947</v>
+        <v>268.28224</v>
       </c>
       <c r="C149">
-        <v>376.99</v>
+        <v>421.85</v>
       </c>
       <c r="D149">
-        <v>97.5</v>
+        <v>57.9</v>
       </c>
       <c r="E149">
-        <v>90.5</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>37529</v>
+        <v>41394</v>
       </c>
       <c r="B150">
-        <v>180.21609620000001</v>
+        <v>255.6112</v>
       </c>
       <c r="C150">
-        <v>378.96</v>
+        <v>421.59</v>
       </c>
       <c r="D150">
-        <v>109.6</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="E150">
-        <v>94.6</v>
+        <v>57.9</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>37499</v>
+        <v>41425</v>
       </c>
       <c r="B151">
-        <v>197.3506442</v>
+        <v>250.23561290000001</v>
       </c>
       <c r="C151">
-        <v>380.34</v>
+        <v>421.74</v>
       </c>
       <c r="D151">
-        <v>116.4</v>
+        <v>78.7</v>
       </c>
       <c r="E151">
-        <v>98.7</v>
+        <v>59.9</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>37468</v>
+        <v>41455</v>
       </c>
       <c r="B152">
-        <v>214.48519229999999</v>
+        <v>231.18559999999999</v>
       </c>
       <c r="C152">
-        <v>382.67</v>
+        <v>422.07</v>
       </c>
       <c r="D152">
-        <v>99.6</v>
+        <v>52.5</v>
       </c>
       <c r="E152">
-        <v>102.7</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>37437</v>
+        <v>41486</v>
       </c>
       <c r="B153">
-        <v>248.7542885</v>
+        <v>224.96432429999999</v>
       </c>
       <c r="C153">
-        <v>384.12</v>
+        <v>422.21</v>
       </c>
       <c r="D153">
-        <v>88.3</v>
+        <v>57</v>
       </c>
       <c r="E153">
-        <v>106.2</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>37389</v>
+        <v>41517</v>
       </c>
       <c r="B154">
-        <v>283.02338459999999</v>
+        <v>269.22890319999999</v>
       </c>
       <c r="C154">
-        <v>386.64</v>
+        <v>421.99</v>
       </c>
       <c r="D154">
-        <v>120.8</v>
+        <v>66</v>
       </c>
       <c r="E154">
-        <v>108.8</v>
+        <v>68.900000000000006</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>37376</v>
+        <v>41547</v>
       </c>
       <c r="B155">
-        <v>180.86293330000001</v>
+        <v>281.25279999999998</v>
       </c>
       <c r="C155">
-        <v>387.62</v>
+        <v>421.79</v>
       </c>
       <c r="D155">
-        <v>120.7</v>
+        <v>37</v>
       </c>
       <c r="E155">
-        <v>110.5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>37346</v>
+        <v>41578</v>
       </c>
       <c r="B156">
-        <v>155.81866669999999</v>
+        <v>273.58864519999997</v>
       </c>
       <c r="C156">
-        <v>389.7</v>
+        <v>421.59</v>
       </c>
       <c r="D156">
-        <v>98.4</v>
+        <v>85.6</v>
       </c>
       <c r="E156">
-        <v>113.3</v>
+        <v>74.900000000000006</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>37315</v>
+        <v>41608</v>
       </c>
       <c r="B157">
-        <v>124.89279999999999</v>
+        <v>266.1829333</v>
       </c>
       <c r="C157">
-        <v>390.83</v>
+        <v>421.98</v>
       </c>
       <c r="D157">
-        <v>107.4</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="E157">
-        <v>114.6</v>
+        <v>75.3</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>37259</v>
+        <v>41639</v>
       </c>
       <c r="B158">
-        <v>202.5226667</v>
+        <v>253.42735479999999</v>
       </c>
       <c r="C158">
-        <v>391.75</v>
+        <v>422.01</v>
       </c>
       <c r="D158">
-        <v>114.1</v>
+        <v>90.3</v>
       </c>
       <c r="E158">
-        <v>113.5</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>37256</v>
+        <v>41670</v>
       </c>
       <c r="B159">
-        <v>248.51741939999999</v>
+        <v>242.15690319999999</v>
       </c>
       <c r="C159">
-        <v>393.53</v>
+        <v>421.91</v>
       </c>
       <c r="D159">
-        <v>132.19999999999999</v>
+        <v>81.8</v>
       </c>
       <c r="E159">
-        <v>114.6</v>
+        <v>77.3</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>37225</v>
+        <v>41698</v>
       </c>
       <c r="B160">
-        <v>313.12639999999999</v>
+        <v>195.16085709999999</v>
       </c>
       <c r="C160">
-        <v>394.66</v>
+        <v>421.24</v>
       </c>
       <c r="D160">
-        <v>106.5</v>
+        <v>102.3</v>
       </c>
       <c r="E160">
-        <v>115.5</v>
+        <v>78.3</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>37195</v>
+        <v>41729</v>
       </c>
       <c r="B161">
-        <v>205.17446150000001</v>
+        <v>249.322</v>
       </c>
       <c r="C161">
-        <v>394.06</v>
+        <v>421.48</v>
       </c>
       <c r="D161">
-        <v>125.5</v>
+        <v>91.9</v>
       </c>
       <c r="E161">
-        <v>114</v>
+        <v>80.8</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>37164</v>
+        <v>41759</v>
       </c>
       <c r="B162">
-        <v>274.27972410000001</v>
+        <v>242.14453330000001</v>
       </c>
       <c r="C162">
-        <v>395.13</v>
+        <v>421.29</v>
       </c>
       <c r="D162">
-        <v>150.69999999999999</v>
+        <v>84.7</v>
       </c>
       <c r="E162">
-        <v>114.1</v>
+        <v>81.900000000000006</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>37134</v>
+        <v>41790</v>
       </c>
       <c r="B163">
-        <v>260.2905806</v>
+        <v>319.72129030000002</v>
       </c>
       <c r="C163">
-        <v>394.73</v>
+        <v>421.41</v>
       </c>
       <c r="D163">
-        <v>106.4</v>
+        <v>75.2</v>
       </c>
       <c r="E163">
-        <v>113.6</v>
+        <v>80.5</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>37103</v>
+        <v>41820</v>
       </c>
       <c r="B164">
-        <v>218.56258059999999</v>
+        <v>249.8898667</v>
       </c>
       <c r="C164">
-        <v>394.24</v>
+        <v>421.48</v>
       </c>
       <c r="D164">
-        <v>81.8</v>
+        <v>71</v>
       </c>
       <c r="E164">
-        <v>111.7</v>
+        <v>79.7</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>37072</v>
+        <v>41851</v>
       </c>
       <c r="B165">
-        <v>200.13120000000001</v>
+        <v>252.98219349999999</v>
       </c>
       <c r="C165">
-        <v>394.57</v>
+        <v>420.86</v>
       </c>
       <c r="D165">
-        <v>134</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="E165">
-        <v>109.8</v>
+        <v>78.599999999999994</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>37042</v>
+        <v>41882</v>
       </c>
       <c r="B166">
-        <v>165.94620689999999</v>
+        <v>259.5852903</v>
       </c>
       <c r="C166">
-        <v>393.85</v>
+        <v>420.94</v>
       </c>
       <c r="D166">
-        <v>96.6</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="E166">
-        <v>108.6</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>37011</v>
+        <v>41912</v>
       </c>
       <c r="B167">
-        <v>262.74568420000003</v>
+        <v>255.61680000000001</v>
       </c>
       <c r="C167">
-        <v>393.57</v>
+        <v>421.91</v>
       </c>
       <c r="D167">
-        <v>107.7</v>
+        <v>87.6</v>
       </c>
       <c r="E167">
-        <v>107.5</v>
+        <v>74.8</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>36978</v>
+        <v>41943</v>
       </c>
       <c r="B168">
-        <v>189.35885709999999</v>
+        <v>241.18038709999999</v>
       </c>
       <c r="C168">
-        <v>393.17</v>
+        <v>421.83</v>
       </c>
       <c r="D168">
-        <v>113.5</v>
+        <v>60.6</v>
       </c>
       <c r="E168">
-        <v>104.8</v>
+        <v>83.4</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>36950</v>
+        <v>41973</v>
       </c>
       <c r="B169">
-        <v>201.38228570000001</v>
+        <v>236.732</v>
       </c>
       <c r="C169">
-        <v>392.5</v>
+        <v>421.13</v>
       </c>
       <c r="D169">
-        <v>80.599999999999994</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="E169">
-        <v>104</v>
+        <v>78.2</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>36922</v>
+        <v>42004</v>
       </c>
       <c r="B170">
-        <v>202.27690319999999</v>
+        <v>201.62425809999999</v>
       </c>
       <c r="C170">
-        <v>392.46</v>
+        <v>421.66500000000002</v>
       </c>
       <c r="D170">
-        <v>95.6</v>
+        <v>78</v>
       </c>
       <c r="E170">
-        <v>108.7</v>
+        <v>81.599999999999994</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>36891</v>
+        <v>42035</v>
       </c>
       <c r="B171">
-        <v>206.46219350000001</v>
+        <v>202.3148387</v>
       </c>
       <c r="C171">
-        <v>392.42</v>
+        <v>422.2</v>
       </c>
       <c r="D171">
-        <v>104.4</v>
+        <v>67</v>
       </c>
       <c r="E171">
-        <v>112</v>
+        <v>72.8</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>36860</v>
+        <v>42052</v>
       </c>
       <c r="B172">
-        <v>415.49381820000002</v>
+        <v>199.51529410000001</v>
       </c>
       <c r="C172">
-        <v>392.17</v>
+        <v>421.74</v>
       </c>
       <c r="D172">
-        <v>106.8</v>
+        <v>72.5</v>
       </c>
       <c r="E172">
-        <v>112.7</v>
+        <v>70.400000000000006</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E172">
+    <sortCondition ref="A2:A172"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>